<commit_message>
Added analysis of prices
</commit_message>
<xml_diff>
--- a/price_history.xlsx
+++ b/price_history.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,21 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>13:07:33</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>25999</v>
       </c>
     </row>
@@ -494,7 +509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +561,36 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>11499</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>13:07:39</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>11499</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22:27:42</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>11499</v>
       </c>
     </row>
@@ -560,7 +605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,6 +657,21 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>20900</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>13:07:47</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>20900</v>
       </c>
     </row>
@@ -626,7 +686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +726,36 @@
         <v>26999</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>13:07:53</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22:27:53</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>26999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>